<commit_message>
Modificacion tipo_comprobante pruebas cobranza por prestaciones
</commit_message>
<xml_diff>
--- a/DBA/Reportes BI/2021/Cobranza por Prestaciones/tipo_comprobante.xlsx
+++ b/DBA/Reportes BI/2021/Cobranza por Prestaciones/tipo_comprobante.xlsx
@@ -443,7 +443,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,7 +552,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -569,7 +569,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -586,7 +586,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>